<commit_message>
attached log to reports
</commit_message>
<xml_diff>
--- a/src/test/java/dataprovider/facebook.xlsx
+++ b/src/test/java/dataprovider/facebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajavenkatasaikiran_\IdeaProjects\TestAutomation\src\test\java\dataprovider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73A805A-F11D-4B48-BCD4-114EE1203FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70FE411-6DCF-447D-AAE5-FF0429C4121B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>kiran@f11</t>
-  </si>
-  <si>
-    <t>kiran@f12</t>
-  </si>
-  <si>
-    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -377,11 +371,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="A4:B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -401,19 +393,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{F5DD4613-0C07-4653-92FC-AC22F39D90E5}"/>
-    <hyperlink ref="A3" r:id="rId2" display="kiran@f11" xr:uid="{888CE326-484B-42B9-AA0F-66C3A994ED62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>